<commit_message>
Analysed experiments from 22-10-05 and 22-10-06
</commit_message>
<xml_diff>
--- a/Data_CalibrationPowerMeter/PowerMeasurements_PMMH.xlsx
+++ b/Data_CalibrationPowerMeter/PowerMeasurements_PMMH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anumi\OneDrive\Desktop\ActinCortexAnalysis\Calibration_PowerMeter_AJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anumi\OneDrive\Desktop\CortExplore\Data_CalibrationPowerMeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Source Filter</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Power measured (uW)</t>
+  </si>
+  <si>
+    <t>area um2</t>
+  </si>
+  <si>
+    <t>uW/um2</t>
+  </si>
+  <si>
+    <t>W/m2</t>
   </si>
 </sst>
 </file>
@@ -350,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,7 +372,7 @@
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -373,8 +382,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -384,8 +402,19 @@
       <c r="C2">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1366</v>
+      </c>
+      <c r="E2">
+        <f>C2/D2</f>
+        <v>1.0468521229868228E-2</v>
+      </c>
+      <c r="F2">
+        <f>E2*10^6</f>
+        <v>10468.521229868229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -395,8 +424,19 @@
       <c r="C3">
         <v>32.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1366</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">C3/D3</f>
+        <v>2.4084919472913614E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">E3*10^6</f>
+        <v>24084.919472913614</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -406,8 +446,19 @@
       <c r="C4">
         <v>66.099999999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1366</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4.8389458272327962E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>48389.45827232796</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -417,8 +468,19 @@
       <c r="C5">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1366</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>9.3704245973645683E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>93704.24597364568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -428,8 +490,19 @@
       <c r="C6">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1366</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.0248901903367497E-4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>102.48901903367498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -439,8 +512,19 @@
       <c r="C7">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1366</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3.7335285505124452E-4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>373.35285505124449</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -450,8 +534,19 @@
       <c r="C8">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1366</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>7.7598828696925329E-4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>775.98828696925329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -461,8 +556,19 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1366</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.4641288433382138E-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1464.1288433382138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -471,6 +577,17 @@
       </c>
       <c r="C10">
         <v>3.7</v>
+      </c>
+      <c r="D10">
+        <v>1366</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2.7086383601756954E-3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2708.6383601756957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>